<commit_message>
updated Measurement Template with concensus suggestions
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/MeasurementTemplateInspectionUpdated.xlsx
+++ b/StateOfPractice/Peter-Notes/MeasurementTemplateInspectionUpdated.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="150">
   <si>
     <t xml:space="preserve">Metrics &amp; Description</t>
   </si>
@@ -52,12 +52,6 @@
     <t xml:space="preserve">(string)</t>
   </si>
   <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
     <t xml:space="preserve">URL?</t>
   </si>
   <si>
@@ -130,54 +124,36 @@
     <t xml:space="preserve">({open source, freeware, commercial, unclear})</t>
   </si>
   <si>
-    <t xml:space="preserve">Publications using the software? Refers to publications that have clearly used the software in their research.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(set of URL or {unclear})</t>
-  </si>
-  <si>
-    <t xml:space="preserve">concern over ability and time required to find all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of instead?</t>
+    <t xml:space="preserve">Publications using the software? Refers to publications that have used the software in their research.</t>
   </si>
   <si>
     <t xml:space="preserve">Publications about the software? Refers to publications that have only mentioned the software and have not clearly applied it.</t>
   </si>
   <si>
-    <t xml:space="preserve">Is source code publicly available?</t>
+    <t xml:space="preserve">Source code URL?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">({set of url, n/a, unclear})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programming language(s)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(set of {FORTRAN, Matlab, C, C++, Java, R, Ruby, Python, Cython, BASIC, Pascal, IDL, unclear, other*}) * given via string </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional comments? (can cover any metrics you feel are missing, or any other thoughts you have)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installability  (Measured via installation on a virtual machine.) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are there installation instructions?</t>
   </si>
   <si>
     <t xml:space="preserve">({yes, no})</t>
   </si>
   <si>
-    <t xml:space="preserve">can we remove this since we have the following question?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source code URL?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">({set of url, n/a, unclear})</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Programming language(s)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(set of {FORTRAN, Matlab, C, C++, Java, R, Ruby, Python, Cython, BASIC, Pascal, IDL, unclear, other*}) * given via string </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional comments? (can cover any metrics you feel are missing, or any other thoughts you have)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Would a question about the software development model (Waterfall, agile, other) be helpful and measurable? 2. Once we settle on the empirical measures, some of them may be measured under this category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Installability  (Measured via installation on a virtual machine.) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are there installation instructions?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Are the installation instructions in one place? Place referring to a single document or web page.</t>
   </si>
   <si>
@@ -202,10 +178,13 @@
     <t xml:space="preserve">({yes∗ , no})</t>
   </si>
   <si>
+    <t xml:space="preserve">If the software installation broke, was a descriptive error message displayed?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Is there a specified way to validate the installation?</t>
   </si>
   <si>
-    <t xml:space="preserve">How many steps were involved in the installation? Including manually unzipping files. Specify OS.</t>
+    <t xml:space="preserve">How many steps were involved in the installation? (Includes manual steps like unzipping files) Specify OS.</t>
   </si>
   <si>
     <t xml:space="preserve">(number, OS)</t>
@@ -217,9 +196,6 @@
     <t xml:space="preserve">({Windows, Linux, OS X, Android, other* }) *given via string</t>
   </si>
   <si>
-    <t xml:space="preserve">should this be a set of</t>
-  </si>
-  <si>
     <t xml:space="preserve">How many software packages need to be installed before or during installation?</t>
   </si>
   <si>
@@ -239,9 +215,6 @@
   </si>
   <si>
     <t xml:space="preserve">({1 .. 10})</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. are there options to repair if software is faulty after installation. </t>
   </si>
   <si>
     <t xml:space="preserve">Correctness and Verifiability</t>
@@ -290,7 +263,13 @@
     <t xml:space="preserve">Does your tutorial output match the expected output?</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Are unit tests available? ({yes, no, unclear})2. Is there evidence of continuous integration? (mentioned in documentation) ({yes, no, unclear})</t>
+    <t xml:space="preserve">Are unit tests available? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there evidence of continuous integration? (for example mentioned in documentation, Jenkins, Travis CI, Bamboo, other)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">({yes*, no, unclear})</t>
   </si>
   <si>
     <t xml:space="preserve">Surface Reliability</t>
@@ -299,9 +278,6 @@
     <t xml:space="preserve">Did the software “break” during installation?</t>
   </si>
   <si>
-    <t xml:space="preserve">If the software installation broke, was a descriptive error message displayed?</t>
-  </si>
-  <si>
     <t xml:space="preserve">If the software installation broke, was the installation instance recoverable?</t>
   </si>
   <si>
@@ -317,9 +293,6 @@
     <t xml:space="preserve">If the tutorial testing broke, was the tutorial testing instance recoverable?</t>
   </si>
   <si>
-    <t xml:space="preserve">consider moving 49-51 to installability</t>
-  </si>
-  <si>
     <t xml:space="preserve">Surface Robustness</t>
   </si>
   <si>
@@ -335,9 +308,6 @@
     <t xml:space="preserve">({yes, no∗ , n/a})</t>
   </si>
   <si>
-    <t xml:space="preserve">We should consider dropping this entirely, and asking the "domain expert" user to give us their impression - a short bit of testing might not be enough to measure robustness</t>
-  </si>
-  <si>
     <t xml:space="preserve">Surface Performance</t>
   </si>
   <si>
@@ -350,6 +320,9 @@
     <t xml:space="preserve">Does the software allow the use of a GPU for processing?</t>
   </si>
   <si>
+    <t xml:space="preserve">We should consider dropping this entirely, and asking the "domain expert" user to give us their impression – this might not be enough to measure performance. Thoughts?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Surface Usability</t>
   </si>
   <si>
@@ -365,10 +338,13 @@
     <t xml:space="preserve">What is the user support model? FAQ? User forum? E-mail address to direct questions? Etc.</t>
   </si>
   <si>
+    <t xml:space="preserve">Need more to measure usablity. Ask domain experts to give us their impression. Thoughts?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maintainability</t>
   </si>
   <si>
-    <t xml:space="preserve">Is there a history of multiple versions of the software? OR How many versions exist (number)</t>
+    <t xml:space="preserve">What is the current version number?</t>
   </si>
   <si>
     <t xml:space="preserve">Is there any information on how code is reviewed, or how to contribute?</t>
@@ -404,7 +380,7 @@
     <t xml:space="preserve">Is there evidence that maintainability was considered in the design? </t>
   </si>
   <si>
-    <t xml:space="preserve">already covered in comments, documents, tracking</t>
+    <t xml:space="preserve">We questioned removing this as it is already covered in comments, documents, tracking. We are leaning towards keeping it as it is a catch all. Old templates did not have anything specific / interesting simply yes or no.</t>
   </si>
   <si>
     <t xml:space="preserve">Reusability</t>
@@ -413,10 +389,7 @@
     <t xml:space="preserve">How many code files are there?</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of classes?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(number or {n/a})</t>
+    <t xml:space="preserve">Is this a good replacement for “Is the system modularized?”</t>
   </si>
   <si>
     <t xml:space="preserve">Is API documented?</t>
@@ -425,9 +398,6 @@
     <t xml:space="preserve">{1 .. 10}</t>
   </si>
   <si>
-    <t xml:space="preserve">Combine maintainability and reusability, since the measures mentioned could apply to both</t>
-  </si>
-  <si>
     <t xml:space="preserve">Portability</t>
   </si>
   <si>
@@ -443,7 +413,7 @@
     <t xml:space="preserve">Convincing evidence that portability has been achieved? </t>
   </si>
   <si>
-    <t xml:space="preserve">Remove?  The platforms the software works on his covered elsewhere, and we aren't going to verify it for all Oss</t>
+    <t xml:space="preserve">Remove?  The platforms the software works on his covered elsewhere, and we aren't going to verify it for all OSs. We are leaning towards removal of portablityfrom the document. Thoughts?</t>
   </si>
   <si>
     <t xml:space="preserve">Surface Understandability (Based on 10 random source files)</t>
@@ -479,13 +449,13 @@
     <t xml:space="preserve">Interoperability</t>
   </si>
   <si>
-    <t xml:space="preserve">Could the software take output from other software as input? (Does the software read input from a file?)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no (how is it determined?)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drop this one entirely, since it doesn't add enough to be worth the effort?</t>
+    <t xml:space="preserve">Does the software produce common extension files as output?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the software use common extension files as input?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop this one entirely, since it doesn't add enough to be worth the effort? Thoughts?</t>
   </si>
   <si>
     <t xml:space="preserve">Visibility/Transparency</t>
@@ -506,7 +476,7 @@
     <t xml:space="preserve">Are there release notes? </t>
   </si>
   <si>
-    <t xml:space="preserve">Better to assess via discussion with developers?</t>
+    <t xml:space="preserve">We will keep this section but note that it is best to ask developers.</t>
   </si>
   <si>
     <t xml:space="preserve">Reproducability</t>
@@ -515,7 +485,7 @@
     <t xml:space="preserve">Is test data available for verification? </t>
   </si>
   <si>
-    <t xml:space="preserve">Could the "domain expert" do a reproducability experiment?</t>
+    <t xml:space="preserve">Could the "domain expert" do a reproducability experiment? Thoughts?</t>
   </si>
 </sst>
 </file>
@@ -571,18 +541,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -653,7 +617,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -686,48 +650,60 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -807,12 +783,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ122"/>
+  <dimension ref="A1:AMJ123"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -862,995 +838,958 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B14" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+    <row r="15" customFormat="false" ht="69.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="B18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="12" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="B20" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+    <row r="21" customFormat="false" ht="75.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
+      <c r="B21" s="8"/>
+    </row>
+    <row r="22" s="6" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B22" s="5"/>
+      <c r="AMJ22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="B23" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+    <row r="24" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B25" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="75.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="11" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" s="6" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+      <c r="B27" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="AMJ23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>59</v>
+      <c r="B29" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>62</v>
+      <c r="A31" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>65</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>73</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B38" s="9"/>
     </row>
     <row r="39" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B39" s="5"/>
       <c r="AMJ39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="73.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>78</v>
-      </c>
+      <c r="A41" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="10"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="46.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="s">
+      <c r="A46" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="48" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="AMJ48" s="0"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="s">
-        <v>88</v>
+    </row>
+    <row r="47" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="46.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="9"/>
+    </row>
+    <row r="50" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="AMJ50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>90</v>
+      <c r="A52" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>53</v>
+      <c r="A53" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B57" s="13"/>
+    </row>
+    <row r="58" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="AMJ58" s="0"/>
+    </row>
+    <row r="59" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="73.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B62" s="13"/>
+    </row>
+    <row r="63" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B63" s="14"/>
+      <c r="AMJ63" s="0"/>
+    </row>
+    <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="s">
+    </row>
+    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B56" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="76.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="AMJ57" s="0"/>
-    </row>
-    <row r="58" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
+    </row>
+    <row r="68" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="73.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="62" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B62" s="16"/>
-      <c r="AMJ62" s="0"/>
-    </row>
-    <row r="63" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="76.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B66" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="67" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B67" s="5"/>
-      <c r="AMJ67" s="0"/>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="B68" s="5"/>
+      <c r="AMJ68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="46.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="AMJ75" s="0"/>
+    </row>
+    <row r="76" customFormat="false" ht="24.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="39.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
+      <c r="B79" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="8" t="s">
+    </row>
+    <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B73" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="74" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="4" t="s">
+      <c r="B80" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B74" s="5"/>
-      <c r="AMJ74" s="0"/>
-    </row>
-    <row r="75" customFormat="false" ht="46.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="11" t="s">
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B75" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
+      <c r="B81" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C81" s="10"/>
+    </row>
+    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B76" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="39.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
+      <c r="B82" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="C82" s="10"/>
+    </row>
+    <row r="83" s="20" customFormat="true" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="19" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
+      <c r="B83" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E83" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="B78" s="8" t="s">
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
+      <c r="B86" s="5"/>
+      <c r="AMJ86" s="0"/>
+    </row>
+    <row r="87" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B87" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" s="21" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E82" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="85" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B85" s="5"/>
-      <c r="AMJ85" s="0"/>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B86" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B87" s="11" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="8" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B90" s="15" t="s">
-        <v>129</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B90" s="13"/>
     </row>
     <row r="91" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B91" s="5"/>
       <c r="AMJ91" s="0"/>
     </row>
     <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>59</v>
+        <v>124</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="53.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B96" s="15" t="s">
-        <v>135</v>
-      </c>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="96" s="10" customFormat="true" ht="70.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E96" s="11"/>
     </row>
     <row r="97" s="6" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B97" s="5"/>
       <c r="AMJ97" s="0"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B100" s="18" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B102" s="18" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B103" s="18" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="108" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B108" s="5"/>
       <c r="AMJ108" s="0"/>
     </row>
-    <row r="109" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="11" t="s">
-        <v>147</v>
+    <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D109" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+      <c r="D109" s="11"/>
+    </row>
+    <row r="110" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B111" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="112" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B112" s="5"/>
-      <c r="AMJ112" s="0"/>
-    </row>
-    <row r="113" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B113" s="18" t="s">
-        <v>152</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D110" s="11"/>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D111" s="10"/>
+    </row>
+    <row r="112" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A112" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B112" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D112" s="10"/>
+    </row>
+    <row r="113" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B113" s="5"/>
+      <c r="AMJ113" s="0"/>
     </row>
     <row r="114" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B114" s="18" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B115" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B116" s="18" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B118" s="15" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="119" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B119" s="5"/>
-      <c r="AMJ119" s="0"/>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B120" s="18" t="s">
-        <v>42</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B117" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A119" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="120" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B120" s="5"/>
+      <c r="AMJ120" s="0"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B122" s="15" t="s">
-        <v>159</v>
+        <v>148</v>
+      </c>
+      <c r="B121" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A123" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B123" s="16" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clarified list or artifacts question under maintainability in MeasurementTemplateInspectionUpdated.xlxs
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/MeasurementTemplateInspectionUpdated.xlsx
+++ b/StateOfPractice/Peter-Notes/MeasurementTemplateInspectionUpdated.xlsx
@@ -339,7 +339,7 @@
     <t xml:space="preserve">Is there any information on how code is reviewed, or how to contribute?</t>
   </si>
   <si>
-    <t xml:space="preserve">Are technical documents available (requirements, architecture, code, algorithms, interfaces, APIs)? </t>
+    <t xml:space="preserve">Are technical documents and artifacts available (functional specs, requirements, SRS, architecture, design, entity relationship diagram, MIS, V&amp;V plans, coding standard docs, algorithms, interfaces, API docs, configuration docs, etc.)? </t>
   </si>
   <si>
     <t xml:space="preserve">({yes*, no, unclear}) *list via string</t>
@@ -539,7 +539,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -580,24 +580,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -620,12 +604,12 @@
   <dimension ref="A1:AMJ103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A104" activeCellId="0" sqref="A104"/>
+      <selection pane="bottomLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.87"/>
@@ -1219,7 +1203,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="39.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="73.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>100</v>
       </c>
@@ -1279,15 +1263,15 @@
       <c r="B81" s="5"/>
       <c r="AMJ81" s="0"/>
     </row>
-    <row r="82" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="10" t="s">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B82" s="10" t="s">
+      <c r="B82" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C82" s="11"/>
-      <c r="E82" s="13"/>
+      <c r="C82" s="10"/>
+      <c r="E82" s="9"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="8" t="s">
@@ -1446,7 +1430,7 @@
       <c r="A103" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B103" s="14"/>
+      <c r="B103" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
clarified artifacts question under maintainability in MeasurementTemplateInspectionUpdated.xlxs
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/MeasurementTemplateInspectionUpdated.xlsx
+++ b/StateOfPractice/Peter-Notes/MeasurementTemplateInspectionUpdated.xlsx
@@ -339,7 +339,7 @@
     <t xml:space="preserve">Is there any information on how code is reviewed, or how to contribute?</t>
   </si>
   <si>
-    <t xml:space="preserve">Are technical documents and artifacts available (functional specs, requirements, SRS, architecture, design, entity relationship diagram, MIS, V&amp;V plans, coding standard docs, algorithms, interfaces, API docs, configuration docs, etc.)? </t>
+    <t xml:space="preserve">Are artifacts available? (List every type of file that is not a code file – for examples please look at the ‘Artifact Name’ column of https://gitlab.cas.mcmaster.ca/SEforSC/se4sc/-/blob/git-svn/GradStudents/Olu/ResearchProposal/Artifacts_MiningV3.xlsx)</t>
   </si>
   <si>
     <t xml:space="preserve">({yes*, no, unclear}) *list via string</t>
@@ -604,14 +604,14 @@
   <dimension ref="A1:AMJ103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
+      <selection pane="bottomLeft" activeCell="A73" activeCellId="0" sqref="A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.83"/>

</xml_diff>